<commit_message>
Add more hints and links to sample form
</commit_message>
<xml_diff>
--- a/extras/Launch WhatsApp.xlsx
+++ b/extras/Launch WhatsApp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cking/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chuck/github/launch-whatsapp/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7374F2-F0FF-C544-A3C7-5CC75FD47490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6F85E1-05BE-8546-862F-9A4CA7729146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33380" yWindow="740" windowWidth="37880" windowHeight="26220" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="help-choices" sheetId="5" r:id="rId5"/>
     <sheet name="help-settings" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -29,7 +29,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5090" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="393">
   <si>
     <t>type</t>
   </si>
@@ -2610,51 +2613,21 @@
     <t>number</t>
   </si>
   <si>
-    <t>Please enter the phone number to which you wish to send an SMS message.</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>message</t>
   </si>
   <si>
     <t>Please enter the message you would like to send.</t>
   </si>
   <si>
-    <t>launch_sms</t>
-  </si>
-  <si>
-    <t>Click the button to send a text message</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>numbers_phone</t>
   </si>
   <si>
-    <t>Launch SMS</t>
-  </si>
-  <si>
-    <t>custom-launch-sms(number=${number},message=${message})</t>
-  </si>
-  <si>
-    <t>+1 555-555-5555</t>
-  </si>
-  <si>
     <t>Hi, I'd like to ask you a few questions.</t>
   </si>
   <si>
-    <t>launch_sms_copy</t>
-  </si>
-  <si>
-    <t>Click the button to send a text message (disabled)</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Launch WhatsApp</t>
   </si>
   <si>
@@ -2664,22 +2637,6 @@
     <t>+15555555555</t>
   </si>
   <si>
-    <t>numbers_phone custom-launch-whatsapp(number=${number}, message=${message})</t>
-  </si>
-  <si>
-    <t>custom-launch-whatsapp(number=${number}, message=${message})</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Please click the button below to launch WhatsApp&lt;/p&gt;
-&lt;div&gt;&lt;small&gt;If WhatsApp is not yet installed on this device, you can &lt;a href="https://www.whatsapp.com/" target="_blank" rel="noopener"&gt;click here to install WhatsApp&lt;/a&gt;.&lt;/small&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>Please enter the phone number of the WhatsApp recipient.</t>
-  </si>
-  <si>
-    <t>You can leave this blank if you'd like the enumerator to select from their own existing list of contacts in WhatsApp.</t>
-  </si>
-  <si>
     <t>Enter the phone number of the WhatsApp recipient.</t>
   </si>
   <si>
@@ -2690,13 +2647,33 @@
   </si>
   <si>
     <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>intronote</t>
+  </si>
+  <si>
+    <t>You can leave this blank if you'd like the enumerator to select from their own existing list of contacts in WhatsApp. 
+Please note: this phone number must be a valid WhatsApp number (i.e. registered to a WhatsApp account) in international format. If you use the default phone number (+15555555555), you will get an error in WhatsApp. Try using your own phone number here instead.</t>
+  </si>
+  <si>
+    <t>If WhatsApp is not yet installed on this device, you can &lt;a href="https://www.whatsapp.com/" target="_blank" rel="noopener"&gt;click here to install WhatsApp&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;h3 style="margin-bottom: 16px"&gt;Welcome to the "Launch WhatsApp" sample form!&lt;/h3&gt;
+&lt;p style="margin-bottom: 16px"&gt;In this sample form, we demonstrate the functionality of the "Launch WhatsApp" field plug-in for SurveyCTO.&lt;/p&gt;
+&lt;p&gt;For more details about this field plug-in, please consult &lt;a href="https://github.com/surveycto/launch-whatsapp/blob/master/README.md" target="_blank" rel="noopener"&gt;the documentation&lt;/a&gt;. If WhatsApp is not yet installed on this device, you can &lt;a href="https://www.whatsapp.com/" target="_blank" rel="noopener"&gt;click here to install WhatsApp&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Please click the button below to launch WhatsApp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2862,7 +2839,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -3025,6 +3002,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3139,7 +3127,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3255,6 +3243,14 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5039,38 +5035,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="9" width="29.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="9" width="19.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="30.5" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="11" width="23.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="9" width="7.1640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="9" width="12.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="9" width="17.1640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="11" width="17.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="9" width="17.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="9" width="8.1640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="9" width="8.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="9" width="18.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="9" width="9.1640625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="9" width="18.33203125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="9" width="13.1640625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="9" width="12.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="9" width="11.6640625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="9" width="11.5" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="9" width="15.0" collapsed="true"/>
-    <col min="20" max="21" customWidth="true" style="9" width="48.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="9" width="10.83203125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="9" width="17.0" collapsed="true"/>
-    <col min="24" max="16384" style="2" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="29" style="9" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.83203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.6640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.5" style="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17" style="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18" style="9" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.1640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.5" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15" style="9" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="48" style="9" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="17" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="11" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5158,7 +5154,7 @@
         <v>358</v>
       </c>
       <c r="V2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5169,7 +5165,7 @@
         <v>9</v>
       </c>
       <c r="V3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5186,7 +5182,7 @@
         <v>358</v>
       </c>
       <c r="V4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5203,7 +5199,7 @@
         <v>358</v>
       </c>
       <c r="V5" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5220,7 +5216,7 @@
         <v>358</v>
       </c>
       <c r="V6" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5237,7 +5233,7 @@
         <v>358</v>
       </c>
       <c r="V7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5254,7 +5250,7 @@
         <v>358</v>
       </c>
       <c r="V8" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5274,7 +5270,7 @@
         <v>293</v>
       </c>
       <c r="V9" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5291,50 +5287,47 @@
         <v>358</v>
       </c>
       <c r="V10" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="204" x14ac:dyDescent="0.2">
+      <c r="A11" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>388</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>391</v>
+      </c>
+      <c r="D11" s="55"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53" t="s">
+        <v>387</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="53"/>
+      <c r="V11"/>
+    </row>
+    <row r="12" spans="1:23" ht="221" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>87</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>374</v>
       </c>
-      <c r="C11" t="s">
-        <v>398</v>
-      </c>
-      <c r="D11" t="s">
-        <v>397</v>
-      </c>
-      <c r="E11" t="s">
-        <v>392</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="C12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>389</v>
+      </c>
+      <c r="E12" t="s">
         <v>382</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="K11" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="E12" t="s">
-        <v>401</v>
+      <c r="F12" t="s">
+        <v>378</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>358</v>
@@ -5343,53 +5336,79 @@
         <v>358</v>
       </c>
       <c r="K12" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>377</v>
+        <v>1</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="E13" t="s">
         <v>386</v>
       </c>
-      <c r="F13" t="s">
+      <c r="I13" s="11" t="s">
         <v>358</v>
       </c>
+      <c r="J13" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="K13" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E14" t="s">
+        <v>379</v>
+      </c>
+      <c r="F14" t="s">
+        <v>358</v>
+      </c>
+      <c r="K14" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" t="s">
-        <v>391</v>
-      </c>
-      <c r="C14" t="s">
-        <v>395</v>
-      </c>
-      <c r="F14" t="s">
-        <v>400</v>
-      </c>
-      <c r="K14" t="s">
-        <v>381</v>
-      </c>
-      <c r="M14" s="9" t="s">
+      <c r="C15" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="F15" t="s">
+        <v>385</v>
+      </c>
+      <c r="K15" t="s">
+        <v>377</v>
+      </c>
+      <c r="M15" s="9" t="s">
         <v>358</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B1:C1048576 I1:I1048576 F1:F10 F12:F1048576">
+  <conditionalFormatting sqref="F1:F11 B1:C1048576 I1:I1048576 F13:F1048576">
     <cfRule type="expression" dxfId="159" priority="75" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
@@ -5399,7 +5418,7 @@
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 F1:F10 F12:F1048576">
+  <conditionalFormatting sqref="F1:F11 B1:D1048576 F13:F1048576">
     <cfRule type="expression" dxfId="157" priority="69" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
@@ -5414,12 +5433,12 @@
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F10 F12:F1048576">
+  <conditionalFormatting sqref="F1:F11 B1:C1048576 F13:F1048576">
     <cfRule type="expression" dxfId="154" priority="60" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F10 B1:B1048576 F12:F1048576">
+  <conditionalFormatting sqref="F1:F11 B1:B1048576 F13:F1048576">
     <cfRule type="expression" dxfId="153" priority="50" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
@@ -5440,12 +5459,12 @@
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F10 F12:F1048576">
+  <conditionalFormatting sqref="F1:F11 B1:C1048576 F13:F1048576">
     <cfRule type="expression" dxfId="148" priority="40" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F10 F12:F1048576">
+  <conditionalFormatting sqref="F1:F11 B1:C1048576 F13:F1048576">
     <cfRule type="expression" dxfId="147" priority="36" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
@@ -5455,7 +5474,7 @@
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W10 A12:W1048576 A11:E11 G11:W11">
+  <conditionalFormatting sqref="A1:W11 A12:E12 G12:W12 A13:W1048576">
     <cfRule type="expression" dxfId="145" priority="28" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
@@ -5519,108 +5538,111 @@
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F10 F12:F1048576">
+  <conditionalFormatting sqref="F1:F11 B1:B1048576 F13:F1048576">
     <cfRule type="expression" dxfId="125" priority="27" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="124" priority="25" stopIfTrue="1">
-      <formula>$A11="begin group"</formula>
+      <formula>$A12="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="123" priority="20" stopIfTrue="1">
-      <formula>$A11="text"</formula>
+      <formula>$A12="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="122" priority="16" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A11, 16)="select_multiple ", LEN($A11)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A11, 17)))), AND(LEFT($A11, 11)="select_one ", LEN($A11)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A11, 12)))))</formula>
+      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="121" priority="13" stopIfTrue="1">
-      <formula>OR($A11="audio audit", $A11="text audit", $A11="speed violations count", $A11="speed violations list", $A11="speed violations audit")</formula>
+      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="120" priority="7" stopIfTrue="1">
-      <formula>OR($A11="date", $A11="datetime")</formula>
+      <formula>OR($A12="date", $A12="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="119" priority="5" stopIfTrue="1">
-      <formula>$A11="image"</formula>
+      <formula>$A12="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="118" priority="2" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A11, 14)="sensor_stream ", LEN($A11)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A11, 15)))), AND(LEFT($A11, 17)="sensor_statistic ", LEN($A11)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A11, 18)))))</formula>
+      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="117" priority="3" stopIfTrue="1">
-      <formula>$A11="comments"</formula>
+      <formula>$A12="comments"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="116" priority="4" stopIfTrue="1">
-      <formula>OR($A11="audio", $A11="video")</formula>
+      <formula>OR($A12="audio", $A12="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="115" priority="6" stopIfTrue="1">
-      <formula>$A11="image"</formula>
+      <formula>$A12="image"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="8" stopIfTrue="1">
-      <formula>OR($A11="date", $A11="datetime")</formula>
+      <formula>OR($A12="date", $A12="datetime")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="113" priority="9" stopIfTrue="1">
-      <formula>OR($A11="calculate", $A11="calculate_here")</formula>
+      <formula>OR($A12="calculate", $A12="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="112" priority="10" stopIfTrue="1">
-      <formula>$A11="note"</formula>
+      <formula>$A12="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="111" priority="11" stopIfTrue="1">
-      <formula>$A11="barcode"</formula>
+      <formula>$A12="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="110" priority="12" stopIfTrue="1">
-      <formula>OR($A11="geopoint", $A11="geoshape", $A11="geotrace")</formula>
+      <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="109" priority="14" stopIfTrue="1">
-      <formula>OR($A11="audio audit", $A11="text audit", $A11="speed violations count", $A11="speed violations list", $A11="speed violations audit")</formula>
+      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="108" priority="15" stopIfTrue="1">
-      <formula>OR($A11="username", $A11="phonenumber", $A11="start", $A11="end", $A11="deviceid", $A11="subscriberid", $A11="simserial", $A11="caseid")</formula>
+      <formula>OR($A12="username", $A12="phonenumber", $A12="start", $A12="end", $A12="deviceid", $A12="subscriberid", $A12="simserial", $A12="caseid")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="107" priority="17" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A11, 16)="select_multiple ", LEN($A11)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A11, 17)))), AND(LEFT($A11, 11)="select_one ", LEN($A11)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A11, 12)))))</formula>
+      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="106" priority="18" stopIfTrue="1">
-      <formula>$A11="decimal"</formula>
+      <formula>$A12="decimal"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="105" priority="19" stopIfTrue="1">
-      <formula>$A11="integer"</formula>
+      <formula>$A12="integer"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="104" priority="21" stopIfTrue="1">
-      <formula>$A11="text"</formula>
+      <formula>$A12="text"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="103" priority="22" stopIfTrue="1">
-      <formula>$A11="end repeat"</formula>
+      <formula>$A12="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="102" priority="23" stopIfTrue="1">
-      <formula>$A11="begin repeat"</formula>
+      <formula>$A12="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="101" priority="24" stopIfTrue="1">
-      <formula>$A11="end group"</formula>
+      <formula>$A12="end group"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="100" priority="26" stopIfTrue="1">
-      <formula>$A11="begin group"</formula>
+      <formula>$A12="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A11, 14)="sensor_stream ", LEN($A11)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A11, 15)))), AND(LEFT($A11, 17)="sensor_statistic ", LEN($A11)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A11, 18)))))</formula>
+      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="E12" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -5635,11 +5657,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="15.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="15" width="14.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="15" width="39.6640625" collapsed="true"/>
-    <col min="4" max="5" style="15" width="10.83203125" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="15.5" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5" style="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.83203125" style="15" collapsed="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5736,17 +5758,17 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5772,14 +5794,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C2" s="17" t="str">
-        <f>TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2104261113</v>
+        <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
+        <v>2104280843</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>
@@ -5808,28 +5830,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="21" width="36.0" collapsed="true"/>
-    <col min="4" max="30" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="1" max="2" width="36" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36" style="21" customWidth="1" collapsed="1"/>
+    <col min="4" max="30" width="36" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="58"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -6023,10 +6045,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="63" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -8816,10 +8838,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="64" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="61"/>
+      <c r="B83" s="65"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -9975,24 +9997,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="1" max="7" width="36" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="58"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -10063,32 +10085,32 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="1" max="6" width="36" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="67"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>